<commit_message>
Add indigenous cases output, revise parallelization, plots and results
</commit_message>
<xml_diff>
--- a/code/cambodia/Project/malaria_framework_20210921.xlsx
+++ b/code/cambodia/Project/malaria_framework_20210921.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\vivax-primaquine-Cambodia\code\cambodia\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3088F2F5-E151-4B59-A3A9-7D8178BFF8C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BEF1DE-C9CE-4232-9B20-D3A2EB4A5AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1485,7 +1485,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1860" uniqueCount="712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1868" uniqueCount="716">
   <si>
     <t>Code Name</t>
   </si>
@@ -3728,6 +3728,18 @@
   </si>
   <si>
     <t xml:space="preserve">365 * ((1-m_prev-m_exp)*m_foi - m_exp*(m_mort + m_incub)  ) </t>
+  </si>
+  <si>
+    <t>indig_cases</t>
+  </si>
+  <si>
+    <t>Indigenous malaria cases (locally acquired)</t>
+  </si>
+  <si>
+    <t>hS:J_inf + hSs:J_inf</t>
+  </si>
+  <si>
+    <t>The number of new malaria infections  (counted at exposed stage) in the susceptible population</t>
   </si>
 </sst>
 </file>
@@ -6370,7 +6382,7 @@
   <dimension ref="A1:AF36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7172,10 +7184,10 @@
   <dimension ref="A1:R182"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D161" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomRight" activeCell="E171" sqref="E171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13952,7 +13964,7 @@
         <v>645</v>
       </c>
       <c r="B166" s="49" t="str">
-        <f t="shared" ref="B166" si="14">IF(ISBLANK(Q166),"",CONCATENATE(Q166,CHAR(10),R166))</f>
+        <f t="shared" ref="B166:B169" si="14">IF(ISBLANK(Q166),"",CONCATENATE(Q166,CHAR(10),R166))</f>
         <v>Malaria test positivity
 Taux de positivité aux tests de paludisme</v>
       </c>
@@ -14006,13 +14018,47 @@
       <c r="O167"/>
       <c r="P167" s="52"/>
     </row>
-    <row r="168" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B168" s="52"/>
-      <c r="P168" s="52"/>
+    <row r="168" spans="1:18" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A168" s="22" t="s">
+        <v>712</v>
+      </c>
+      <c r="B168" s="49" t="str">
+        <f t="shared" si="14"/>
+        <v>Indigenous malaria cases (locally acquired)
+TBD</v>
+      </c>
+      <c r="C168" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E168" s="22">
+        <v>0</v>
+      </c>
+      <c r="F168" s="22">
+        <v>0</v>
+      </c>
+      <c r="H168" s="22" t="s">
+        <v>714</v>
+      </c>
+      <c r="I168" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="M168" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="P168" s="52" t="s">
+        <v>715</v>
+      </c>
+      <c r="Q168" s="5" t="s">
+        <v>713</v>
+      </c>
+      <c r="R168" s="22" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="169" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B169" s="52"/>
+      <c r="B169" s="49"/>
       <c r="P169" s="52"/>
+      <c r="Q169" s="5"/>
     </row>
     <row r="170" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B170" s="52"/>

</xml_diff>